<commit_message>
Added key to formatted results
</commit_message>
<xml_diff>
--- a/submissions/lab2/results formatted.xlsx
+++ b/submissions/lab2/results formatted.xlsx
@@ -5,29 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ethan\Documents\GitHub\CSC382-Algorithms-Labs\submissions\lab2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Documents\GitHub\CSC382-Algorithms-Labs\submissions\lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1DAD20-FD70-4F7D-91CE-847FF5A5B363}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C4405E-F965-4103-8922-B3C603BB0D11}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results formatted" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
   <si>
     <t>BOUNDS</t>
   </si>
@@ -66,6 +59,21 @@
   </si>
   <si>
     <t>HEAP SORT: STEPS</t>
+  </si>
+  <si>
+    <t>RAND = array containing N random values from 1 to N</t>
+  </si>
+  <si>
+    <t>PERM = a shuffled array containing N values from 1 to N</t>
+  </si>
+  <si>
+    <t>DEC = decreasing array containing N values from N to 1</t>
+  </si>
+  <si>
+    <t>INC = increasing array containing N values from 1 to N</t>
+  </si>
+  <si>
+    <t>Key:</t>
   </si>
 </sst>
 </file>
@@ -389,7 +397,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -545,6 +553,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -590,7 +607,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2"/>
@@ -600,6 +617,8 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="9" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="25" borderId="10" xfId="34" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="29" borderId="10" xfId="38" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -738,7 +757,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'results formatted'!$A$4</c:f>
+              <c:f>'results formatted'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -761,7 +780,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'results formatted'!$B$3:$I$3</c:f>
+              <c:f>'results formatted'!$B$4:$I$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -794,7 +813,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'results formatted'!$B$4:$I$4</c:f>
+              <c:f>'results formatted'!$B$5:$I$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -837,7 +856,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'results formatted'!$A$5</c:f>
+              <c:f>'results formatted'!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -860,7 +879,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'results formatted'!$B$3:$I$3</c:f>
+              <c:f>'results formatted'!$B$4:$I$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -893,7 +912,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'results formatted'!$B$5:$I$5</c:f>
+              <c:f>'results formatted'!$B$6:$I$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -936,7 +955,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'results formatted'!$A$6</c:f>
+              <c:f>'results formatted'!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -959,7 +978,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'results formatted'!$B$3:$I$3</c:f>
+              <c:f>'results formatted'!$B$4:$I$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -992,7 +1011,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'results formatted'!$B$6:$I$6</c:f>
+              <c:f>'results formatted'!$B$7:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1035,7 +1054,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'results formatted'!$A$7</c:f>
+              <c:f>'results formatted'!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1058,7 +1077,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'results formatted'!$B$3:$I$3</c:f>
+              <c:f>'results formatted'!$B$4:$I$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1091,7 +1110,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'results formatted'!$B$7:$I$7</c:f>
+              <c:f>'results formatted'!$B$8:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1411,7 +1430,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'results formatted'!$K$4</c:f>
+              <c:f>'results formatted'!$K$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1434,7 +1453,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'results formatted'!$L$3:$S$3</c:f>
+              <c:f>'results formatted'!$L$4:$S$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1467,7 +1486,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'results formatted'!$L$4:$S$4</c:f>
+              <c:f>'results formatted'!$L$5:$S$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1510,7 +1529,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'results formatted'!$K$5</c:f>
+              <c:f>'results formatted'!$K$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1533,7 +1552,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'results formatted'!$L$3:$S$3</c:f>
+              <c:f>'results formatted'!$L$4:$S$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1566,7 +1585,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'results formatted'!$L$5:$S$5</c:f>
+              <c:f>'results formatted'!$L$6:$S$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1609,7 +1628,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'results formatted'!$K$6</c:f>
+              <c:f>'results formatted'!$K$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1632,7 +1651,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'results formatted'!$L$3:$S$3</c:f>
+              <c:f>'results formatted'!$L$4:$S$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1665,7 +1684,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'results formatted'!$L$6:$S$6</c:f>
+              <c:f>'results formatted'!$L$7:$S$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1708,7 +1727,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'results formatted'!$K$7</c:f>
+              <c:f>'results formatted'!$K$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1731,7 +1750,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'results formatted'!$L$3:$S$3</c:f>
+              <c:f>'results formatted'!$L$4:$S$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1764,7 +1783,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'results formatted'!$L$7:$S$7</c:f>
+              <c:f>'results formatted'!$L$8:$S$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3123,13 +3142,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3159,13 +3178,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>547687</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>242887</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3491,10 +3510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:S38"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S35" sqref="L35:S36"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="76" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3503,946 +3522,990 @@
     <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B4" s="6">
         <v>100</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C4" s="6">
         <v>200</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D4" s="6">
         <v>300</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E4" s="6">
         <v>400</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F4" s="6">
         <v>500</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G4" s="6">
         <v>1000</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H4" s="6">
         <v>4000</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I4" s="6">
         <v>10000</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L4" s="6">
         <v>100</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M4" s="6">
         <v>200</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N4" s="6">
         <v>300</v>
       </c>
-      <c r="O3" s="6">
+      <c r="O4" s="6">
         <v>400</v>
       </c>
-      <c r="P3" s="6">
+      <c r="P4" s="6">
         <v>500</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="Q4" s="6">
         <v>1000</v>
       </c>
-      <c r="R3" s="6">
+      <c r="R4" s="6">
         <v>4000</v>
       </c>
-      <c r="S3" s="6">
+      <c r="S4" s="6">
         <v>10000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7">
-        <v>27545</v>
-      </c>
-      <c r="C4" s="7">
-        <v>15052</v>
-      </c>
-      <c r="D4" s="7">
-        <v>36581</v>
-      </c>
-      <c r="E4" s="7">
-        <v>80540</v>
-      </c>
-      <c r="F4" s="7">
-        <v>147270</v>
-      </c>
-      <c r="G4" s="7">
-        <v>554427</v>
-      </c>
-      <c r="H4" s="7">
-        <v>8697991</v>
-      </c>
-      <c r="I4" s="7">
-        <v>44553834</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" s="8">
-        <v>10708</v>
-      </c>
-      <c r="M4" s="8">
-        <v>10122</v>
-      </c>
-      <c r="N4" s="8">
-        <v>6582</v>
-      </c>
-      <c r="O4" s="8">
-        <v>10157</v>
-      </c>
-      <c r="P4" s="8">
-        <v>12395</v>
-      </c>
-      <c r="Q4" s="8">
-        <v>35567</v>
-      </c>
-      <c r="R4" s="8">
-        <v>175352</v>
-      </c>
-      <c r="S4" s="8">
-        <v>461433</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="7">
-        <v>33323</v>
+        <v>27545</v>
       </c>
       <c r="C5" s="7">
-        <v>15403</v>
+        <v>15052</v>
       </c>
       <c r="D5" s="7">
-        <v>32943</v>
+        <v>36581</v>
       </c>
       <c r="E5" s="7">
-        <v>56193</v>
+        <v>80540</v>
       </c>
       <c r="F5" s="7">
-        <v>146549</v>
+        <v>147270</v>
       </c>
       <c r="G5" s="7">
-        <v>328367</v>
+        <v>554427</v>
       </c>
       <c r="H5" s="7">
-        <v>5510309</v>
+        <v>8697991</v>
       </c>
       <c r="I5" s="7">
-        <v>31071447</v>
+        <v>44553834</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L5" s="8">
-        <v>5836</v>
+        <v>10708</v>
       </c>
       <c r="M5" s="8">
-        <v>3725</v>
+        <v>10122</v>
       </c>
       <c r="N5" s="8">
-        <v>5831</v>
+        <v>6582</v>
       </c>
       <c r="O5" s="8">
-        <v>10981</v>
+        <v>10157</v>
       </c>
       <c r="P5" s="8">
-        <v>9966</v>
+        <v>12395</v>
       </c>
       <c r="Q5" s="8">
-        <v>33679</v>
+        <v>35567</v>
       </c>
       <c r="R5" s="8">
-        <v>177537</v>
+        <v>175352</v>
       </c>
       <c r="S5" s="8">
-        <v>470927</v>
+        <v>461433</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="7">
-        <v>4203</v>
+        <v>33323</v>
       </c>
       <c r="C6" s="7">
-        <v>6919</v>
+        <v>15403</v>
       </c>
       <c r="D6" s="7">
-        <v>10425</v>
+        <v>32943</v>
       </c>
       <c r="E6" s="7">
-        <v>14218</v>
+        <v>56193</v>
       </c>
       <c r="F6" s="7">
-        <v>23283</v>
+        <v>146549</v>
       </c>
       <c r="G6" s="7">
-        <v>44188</v>
+        <v>328367</v>
       </c>
       <c r="H6" s="7">
-        <v>184729</v>
+        <v>5510309</v>
       </c>
       <c r="I6" s="7">
-        <v>514140</v>
+        <v>31071447</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L6" s="8">
-        <v>7787</v>
+        <v>5836</v>
       </c>
       <c r="M6" s="8">
-        <v>8777</v>
+        <v>3725</v>
       </c>
       <c r="N6" s="8">
-        <v>14326</v>
+        <v>5831</v>
       </c>
       <c r="O6" s="8">
-        <v>20582</v>
+        <v>10981</v>
       </c>
       <c r="P6" s="8">
-        <v>23512</v>
+        <v>9966</v>
       </c>
       <c r="Q6" s="8">
-        <v>52072</v>
+        <v>33679</v>
       </c>
       <c r="R6" s="8">
-        <v>251952</v>
+        <v>177537</v>
       </c>
       <c r="S6" s="8">
-        <v>685290</v>
+        <v>470927</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="7">
+        <v>4203</v>
+      </c>
+      <c r="C7" s="7">
+        <v>6919</v>
+      </c>
+      <c r="D7" s="7">
+        <v>10425</v>
+      </c>
+      <c r="E7" s="7">
+        <v>14218</v>
+      </c>
+      <c r="F7" s="7">
+        <v>23283</v>
+      </c>
+      <c r="G7" s="7">
+        <v>44188</v>
+      </c>
+      <c r="H7" s="7">
+        <v>184729</v>
+      </c>
+      <c r="I7" s="7">
+        <v>514140</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="8">
+        <v>7787</v>
+      </c>
+      <c r="M7" s="8">
+        <v>8777</v>
+      </c>
+      <c r="N7" s="8">
+        <v>14326</v>
+      </c>
+      <c r="O7" s="8">
+        <v>20582</v>
+      </c>
+      <c r="P7" s="8">
+        <v>23512</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>52072</v>
+      </c>
+      <c r="R7" s="8">
+        <v>251952</v>
+      </c>
+      <c r="S7" s="8">
+        <v>685290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B8" s="7">
         <v>2891</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C8" s="7">
         <v>6065</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D8" s="7">
         <v>9869</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E8" s="7">
         <v>15145</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F8" s="7">
         <v>23864</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G8" s="7">
         <v>39199</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H8" s="7">
         <v>188845</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I8" s="7">
         <v>510064</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L8" s="8">
         <v>5958</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M8" s="8">
         <v>8694</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N8" s="8">
         <v>14575</v>
       </c>
-      <c r="O7" s="8">
+      <c r="O8" s="8">
         <v>21191</v>
       </c>
-      <c r="P7" s="8">
+      <c r="P8" s="8">
         <v>24536</v>
       </c>
-      <c r="Q7" s="8">
+      <c r="Q8" s="8">
         <v>52043</v>
       </c>
-      <c r="R7" s="8">
+      <c r="R8" s="8">
         <v>248251</v>
       </c>
-      <c r="S7" s="8">
+      <c r="S8" s="8">
         <v>737996</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
+    <row r="26" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="K26" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B27" s="6">
         <v>100</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C27" s="6">
         <v>200</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D27" s="6">
         <v>300</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E27" s="6">
         <v>400</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F27" s="6">
         <v>500</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G27" s="6">
         <v>1000</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H27" s="6">
         <v>4000</v>
       </c>
-      <c r="I26" s="6">
+      <c r="I27" s="6">
         <v>10000</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L26" s="6">
+      <c r="L27" s="6">
         <v>100</v>
       </c>
-      <c r="M26" s="6">
+      <c r="M27" s="6">
         <v>200</v>
       </c>
-      <c r="N26" s="6">
+      <c r="N27" s="6">
         <v>300</v>
       </c>
-      <c r="O26" s="6">
+      <c r="O27" s="6">
         <v>400</v>
       </c>
-      <c r="P26" s="6">
+      <c r="P27" s="6">
         <v>500</v>
       </c>
-      <c r="Q26" s="6">
+      <c r="Q27" s="6">
         <v>1000</v>
       </c>
-      <c r="R26" s="6">
+      <c r="R27" s="6">
         <v>4000</v>
       </c>
-      <c r="S26" s="6">
+      <c r="S27" s="6">
         <v>10000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="7">
-        <v>35740</v>
-      </c>
-      <c r="C27" s="7">
-        <v>141490</v>
-      </c>
-      <c r="D27" s="7">
-        <v>317240</v>
-      </c>
-      <c r="E27" s="7">
-        <v>562990</v>
-      </c>
-      <c r="F27" s="7">
-        <v>878740</v>
-      </c>
-      <c r="G27" s="7">
-        <v>3507490</v>
-      </c>
-      <c r="H27" s="7">
-        <v>56029990</v>
-      </c>
-      <c r="I27" s="7">
-        <v>350074990</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="L27" s="8">
-        <v>11015</v>
-      </c>
-      <c r="M27" s="8">
-        <v>25445</v>
-      </c>
-      <c r="N27" s="8">
-        <v>41075</v>
-      </c>
-      <c r="O27" s="8">
-        <v>57404</v>
-      </c>
-      <c r="P27" s="8">
-        <v>74089</v>
-      </c>
-      <c r="Q27" s="8">
-        <v>164769</v>
-      </c>
-      <c r="R27" s="8">
-        <v>795955</v>
-      </c>
-      <c r="S27" s="8">
-        <v>2220491</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B28" s="7">
-        <v>25740</v>
+        <v>35740</v>
       </c>
       <c r="C28" s="7">
-        <v>101490</v>
+        <v>141490</v>
       </c>
       <c r="D28" s="7">
-        <v>227240</v>
+        <v>317240</v>
       </c>
       <c r="E28" s="7">
-        <v>402990</v>
+        <v>562990</v>
       </c>
       <c r="F28" s="7">
-        <v>628740</v>
+        <v>878740</v>
       </c>
       <c r="G28" s="7">
-        <v>2507490</v>
+        <v>3507490</v>
       </c>
       <c r="H28" s="7">
-        <v>40029990</v>
+        <v>56029990</v>
       </c>
       <c r="I28" s="7">
-        <v>250074990</v>
+        <v>350074990</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L28" s="8">
-        <v>9032</v>
+        <v>11015</v>
       </c>
       <c r="M28" s="8">
-        <v>20968</v>
+        <v>25445</v>
       </c>
       <c r="N28" s="8">
-        <v>34468</v>
+        <v>41075</v>
       </c>
       <c r="O28" s="8">
-        <v>48656</v>
+        <v>57404</v>
       </c>
       <c r="P28" s="8">
-        <v>63301</v>
+        <v>74089</v>
       </c>
       <c r="Q28" s="8">
-        <v>142432</v>
+        <v>164769</v>
       </c>
       <c r="R28" s="8">
-        <v>704395</v>
+        <v>795955</v>
       </c>
       <c r="S28" s="8">
-        <v>1977368</v>
+        <v>2220491</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B29" s="7">
-        <v>3957</v>
+        <v>25740</v>
       </c>
       <c r="C29" s="7">
-        <v>9382</v>
+        <v>101490</v>
       </c>
       <c r="D29" s="7">
-        <v>15312</v>
+        <v>227240</v>
       </c>
       <c r="E29" s="7">
-        <v>21133</v>
+        <v>402990</v>
       </c>
       <c r="F29" s="7">
-        <v>27533</v>
+        <v>628740</v>
       </c>
       <c r="G29" s="7">
-        <v>62147</v>
+        <v>2507490</v>
       </c>
       <c r="H29" s="7">
-        <v>301665</v>
+        <v>40029990</v>
       </c>
       <c r="I29" s="7">
-        <v>848415</v>
+        <v>250074990</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L29" s="8">
-        <v>10066</v>
+        <v>9032</v>
       </c>
       <c r="M29" s="8">
-        <v>23396</v>
+        <v>20968</v>
       </c>
       <c r="N29" s="8">
-        <v>37883</v>
+        <v>34468</v>
       </c>
       <c r="O29" s="8">
-        <v>53331</v>
+        <v>48656</v>
       </c>
       <c r="P29" s="8">
-        <v>69027</v>
+        <v>63301</v>
       </c>
       <c r="Q29" s="8">
-        <v>154614</v>
+        <v>142432</v>
       </c>
       <c r="R29" s="8">
-        <v>750351</v>
+        <v>704395</v>
       </c>
       <c r="S29" s="8">
-        <v>2096555</v>
+        <v>1977368</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="7">
+        <v>3957</v>
+      </c>
+      <c r="C30" s="7">
+        <v>9382</v>
+      </c>
+      <c r="D30" s="7">
+        <v>15312</v>
+      </c>
+      <c r="E30" s="7">
+        <v>21133</v>
+      </c>
+      <c r="F30" s="7">
+        <v>27533</v>
+      </c>
+      <c r="G30" s="7">
+        <v>62147</v>
+      </c>
+      <c r="H30" s="7">
+        <v>301665</v>
+      </c>
+      <c r="I30" s="7">
+        <v>848415</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L30" s="8">
+        <v>10066</v>
+      </c>
+      <c r="M30" s="8">
+        <v>23396</v>
+      </c>
+      <c r="N30" s="8">
+        <v>37883</v>
+      </c>
+      <c r="O30" s="8">
+        <v>53331</v>
+      </c>
+      <c r="P30" s="8">
+        <v>69027</v>
+      </c>
+      <c r="Q30" s="8">
+        <v>154614</v>
+      </c>
+      <c r="R30" s="8">
+        <v>750351</v>
+      </c>
+      <c r="S30" s="8">
+        <v>2096555</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B31" s="7">
         <v>4085</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C31" s="7">
         <v>9490</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D31" s="7">
         <v>15657</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E31" s="7">
         <v>21730</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F31" s="7">
         <v>28454</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G31" s="7">
         <v>63292</v>
       </c>
-      <c r="H30" s="7">
+      <c r="H31" s="7">
         <v>308037</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I31" s="7">
         <v>864129</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L30" s="8">
+      <c r="L31" s="8">
         <v>10052</v>
       </c>
-      <c r="M30" s="8">
+      <c r="M31" s="8">
         <v>23418</v>
       </c>
-      <c r="N30" s="8">
+      <c r="N31" s="8">
         <v>37861</v>
       </c>
-      <c r="O30" s="8">
+      <c r="O31" s="8">
         <v>53326</v>
       </c>
-      <c r="P30" s="8">
+      <c r="P31" s="8">
         <v>69061</v>
       </c>
-      <c r="Q30" s="8">
+      <c r="Q31" s="8">
         <v>154554</v>
       </c>
-      <c r="R30" s="8">
+      <c r="R31" s="8">
         <v>750101</v>
       </c>
-      <c r="S30" s="8">
+      <c r="S31" s="8">
         <v>2096336</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
+    <row r="34" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F33" s="3"/>
-      <c r="H33" s="4" t="s">
+      <c r="F34" s="3"/>
+      <c r="H34" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I33" s="4"/>
-      <c r="K33" s="2" t="s">
+      <c r="I34" s="4"/>
+      <c r="K34" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="O33" s="3" t="s">
+      <c r="O34" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P33" s="3"/>
-      <c r="R33" s="4" t="s">
+      <c r="P34" s="3"/>
+      <c r="R34" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="S33" s="4"/>
+      <c r="S34" s="4"/>
     </row>
-    <row r="34" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B35" s="6">
         <v>100</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C35" s="6">
         <v>200</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D35" s="6">
         <v>300</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E35" s="6">
         <v>400</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F35" s="6">
         <v>500</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G35" s="6">
         <v>1000</v>
       </c>
-      <c r="H34" s="6">
+      <c r="H35" s="6">
         <v>4000</v>
       </c>
-      <c r="I34" s="6">
+      <c r="I35" s="6">
         <v>10000</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L34" s="6">
+      <c r="L35" s="6">
         <v>100</v>
       </c>
-      <c r="M34" s="6">
+      <c r="M35" s="6">
         <v>200</v>
       </c>
-      <c r="N34" s="6">
+      <c r="N35" s="6">
         <v>300</v>
       </c>
-      <c r="O34" s="6">
+      <c r="O35" s="6">
         <v>400</v>
       </c>
-      <c r="P34" s="6">
+      <c r="P35" s="6">
         <v>500</v>
       </c>
-      <c r="Q34" s="6">
+      <c r="Q35" s="6">
         <v>1000</v>
       </c>
-      <c r="R34" s="6">
+      <c r="R35" s="6">
         <v>4000</v>
       </c>
-      <c r="S34" s="6">
+      <c r="S35" s="6">
         <v>10000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" s="8">
-        <f t="shared" ref="B35:I38" si="0">MIN(B4, L4)</f>
-        <v>10708</v>
-      </c>
-      <c r="C35" s="8">
-        <f t="shared" si="0"/>
-        <v>10122</v>
-      </c>
-      <c r="D35" s="8">
-        <f t="shared" si="0"/>
-        <v>6582</v>
-      </c>
-      <c r="E35" s="8">
-        <f t="shared" si="0"/>
-        <v>10157</v>
-      </c>
-      <c r="F35" s="8">
-        <f t="shared" si="0"/>
-        <v>12395</v>
-      </c>
-      <c r="G35" s="8">
-        <f t="shared" si="0"/>
-        <v>35567</v>
-      </c>
-      <c r="H35" s="8">
-        <f t="shared" si="0"/>
-        <v>175352</v>
-      </c>
-      <c r="I35" s="8">
-        <f t="shared" si="0"/>
-        <v>461433</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="L35" s="8">
-        <f>MIN(B27, L27)</f>
-        <v>11015</v>
-      </c>
-      <c r="M35" s="8">
-        <f t="shared" ref="M35:S35" si="1">MIN(C27, M27)</f>
-        <v>25445</v>
-      </c>
-      <c r="N35" s="8">
-        <f t="shared" si="1"/>
-        <v>41075</v>
-      </c>
-      <c r="O35" s="8">
-        <f t="shared" si="1"/>
-        <v>57404</v>
-      </c>
-      <c r="P35" s="8">
-        <f t="shared" si="1"/>
-        <v>74089</v>
-      </c>
-      <c r="Q35" s="8">
-        <f t="shared" si="1"/>
-        <v>164769</v>
-      </c>
-      <c r="R35" s="8">
-        <f t="shared" si="1"/>
-        <v>795955</v>
-      </c>
-      <c r="S35" s="8">
-        <f t="shared" si="1"/>
-        <v>2220491</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B36" s="8">
-        <f t="shared" si="0"/>
-        <v>5836</v>
+        <f t="shared" ref="B36:I39" si="0">MIN(B5, L5)</f>
+        <v>10708</v>
       </c>
       <c r="C36" s="8">
         <f t="shared" si="0"/>
-        <v>3725</v>
+        <v>10122</v>
       </c>
       <c r="D36" s="8">
         <f t="shared" si="0"/>
-        <v>5831</v>
+        <v>6582</v>
       </c>
       <c r="E36" s="8">
         <f t="shared" si="0"/>
-        <v>10981</v>
+        <v>10157</v>
       </c>
       <c r="F36" s="8">
         <f t="shared" si="0"/>
-        <v>9966</v>
+        <v>12395</v>
       </c>
       <c r="G36" s="8">
         <f t="shared" si="0"/>
-        <v>33679</v>
+        <v>35567</v>
       </c>
       <c r="H36" s="8">
         <f t="shared" si="0"/>
-        <v>177537</v>
+        <v>175352</v>
       </c>
       <c r="I36" s="8">
         <f t="shared" si="0"/>
-        <v>470927</v>
+        <v>461433</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L36" s="8">
-        <f t="shared" ref="L36:S36" si="2">MIN(B28, L28)</f>
-        <v>9032</v>
+        <f>MIN(B28, L28)</f>
+        <v>11015</v>
       </c>
       <c r="M36" s="8">
-        <f t="shared" si="2"/>
-        <v>20968</v>
+        <f t="shared" ref="M36:S36" si="1">MIN(C28, M28)</f>
+        <v>25445</v>
       </c>
       <c r="N36" s="8">
-        <f t="shared" si="2"/>
-        <v>34468</v>
+        <f t="shared" si="1"/>
+        <v>41075</v>
       </c>
       <c r="O36" s="8">
-        <f t="shared" si="2"/>
-        <v>48656</v>
+        <f t="shared" si="1"/>
+        <v>57404</v>
       </c>
       <c r="P36" s="8">
-        <f t="shared" si="2"/>
-        <v>63301</v>
+        <f t="shared" si="1"/>
+        <v>74089</v>
       </c>
       <c r="Q36" s="8">
-        <f t="shared" si="2"/>
-        <v>142432</v>
+        <f t="shared" si="1"/>
+        <v>164769</v>
       </c>
       <c r="R36" s="8">
-        <f t="shared" si="2"/>
-        <v>704395</v>
+        <f t="shared" si="1"/>
+        <v>795955</v>
       </c>
       <c r="S36" s="8">
-        <f t="shared" si="2"/>
-        <v>1977368</v>
+        <f t="shared" si="1"/>
+        <v>2220491</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B37" s="7">
+        <v>2</v>
+      </c>
+      <c r="B37" s="8">
         <f t="shared" si="0"/>
-        <v>4203</v>
-      </c>
-      <c r="C37" s="7">
+        <v>5836</v>
+      </c>
+      <c r="C37" s="8">
         <f t="shared" si="0"/>
-        <v>6919</v>
-      </c>
-      <c r="D37" s="7">
+        <v>3725</v>
+      </c>
+      <c r="D37" s="8">
         <f t="shared" si="0"/>
-        <v>10425</v>
-      </c>
-      <c r="E37" s="7">
+        <v>5831</v>
+      </c>
+      <c r="E37" s="8">
         <f t="shared" si="0"/>
-        <v>14218</v>
-      </c>
-      <c r="F37" s="7">
+        <v>10981</v>
+      </c>
+      <c r="F37" s="8">
         <f t="shared" si="0"/>
-        <v>23283</v>
-      </c>
-      <c r="G37" s="7">
+        <v>9966</v>
+      </c>
+      <c r="G37" s="8">
         <f t="shared" si="0"/>
-        <v>44188</v>
-      </c>
-      <c r="H37" s="7">
+        <v>33679</v>
+      </c>
+      <c r="H37" s="8">
         <f t="shared" si="0"/>
-        <v>184729</v>
-      </c>
-      <c r="I37" s="7">
+        <v>177537</v>
+      </c>
+      <c r="I37" s="8">
         <f t="shared" si="0"/>
-        <v>514140</v>
+        <v>470927</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="L37" s="7">
-        <f t="shared" ref="L37:S37" si="3">MIN(B29, L29)</f>
-        <v>3957</v>
-      </c>
-      <c r="M37" s="7">
-        <f t="shared" si="3"/>
-        <v>9382</v>
-      </c>
-      <c r="N37" s="7">
-        <f t="shared" si="3"/>
-        <v>15312</v>
-      </c>
-      <c r="O37" s="7">
-        <f>MIN(E29, O29)</f>
-        <v>21133</v>
-      </c>
-      <c r="P37" s="7">
-        <f t="shared" si="3"/>
-        <v>27533</v>
-      </c>
-      <c r="Q37" s="7">
-        <f t="shared" si="3"/>
-        <v>62147</v>
-      </c>
-      <c r="R37" s="7">
-        <f t="shared" si="3"/>
-        <v>301665</v>
-      </c>
-      <c r="S37" s="7">
-        <f t="shared" si="3"/>
-        <v>848415</v>
+        <v>2</v>
+      </c>
+      <c r="L37" s="8">
+        <f t="shared" ref="L37:S37" si="2">MIN(B29, L29)</f>
+        <v>9032</v>
+      </c>
+      <c r="M37" s="8">
+        <f t="shared" si="2"/>
+        <v>20968</v>
+      </c>
+      <c r="N37" s="8">
+        <f t="shared" si="2"/>
+        <v>34468</v>
+      </c>
+      <c r="O37" s="8">
+        <f t="shared" si="2"/>
+        <v>48656</v>
+      </c>
+      <c r="P37" s="8">
+        <f t="shared" si="2"/>
+        <v>63301</v>
+      </c>
+      <c r="Q37" s="8">
+        <f t="shared" si="2"/>
+        <v>142432</v>
+      </c>
+      <c r="R37" s="8">
+        <f t="shared" si="2"/>
+        <v>704395</v>
+      </c>
+      <c r="S37" s="8">
+        <f t="shared" si="2"/>
+        <v>1977368</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B38" s="7">
         <f t="shared" si="0"/>
-        <v>2891</v>
+        <v>4203</v>
       </c>
       <c r="C38" s="7">
         <f t="shared" si="0"/>
-        <v>6065</v>
+        <v>6919</v>
       </c>
       <c r="D38" s="7">
         <f t="shared" si="0"/>
-        <v>9869</v>
+        <v>10425</v>
       </c>
       <c r="E38" s="7">
         <f t="shared" si="0"/>
-        <v>15145</v>
+        <v>14218</v>
       </c>
       <c r="F38" s="7">
         <f t="shared" si="0"/>
-        <v>23864</v>
+        <v>23283</v>
       </c>
       <c r="G38" s="7">
         <f t="shared" si="0"/>
-        <v>39199</v>
+        <v>44188</v>
       </c>
       <c r="H38" s="7">
         <f t="shared" si="0"/>
-        <v>188845</v>
+        <v>184729</v>
       </c>
       <c r="I38" s="7">
         <f t="shared" si="0"/>
+        <v>514140</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L38" s="7">
+        <f t="shared" ref="L38:S38" si="3">MIN(B30, L30)</f>
+        <v>3957</v>
+      </c>
+      <c r="M38" s="7">
+        <f t="shared" si="3"/>
+        <v>9382</v>
+      </c>
+      <c r="N38" s="7">
+        <f t="shared" si="3"/>
+        <v>15312</v>
+      </c>
+      <c r="O38" s="7">
+        <f>MIN(E30, O30)</f>
+        <v>21133</v>
+      </c>
+      <c r="P38" s="7">
+        <f t="shared" si="3"/>
+        <v>27533</v>
+      </c>
+      <c r="Q38" s="7">
+        <f t="shared" si="3"/>
+        <v>62147</v>
+      </c>
+      <c r="R38" s="7">
+        <f t="shared" si="3"/>
+        <v>301665</v>
+      </c>
+      <c r="S38" s="7">
+        <f t="shared" si="3"/>
+        <v>848415</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="7">
+        <f t="shared" si="0"/>
+        <v>2891</v>
+      </c>
+      <c r="C39" s="7">
+        <f t="shared" si="0"/>
+        <v>6065</v>
+      </c>
+      <c r="D39" s="7">
+        <f t="shared" si="0"/>
+        <v>9869</v>
+      </c>
+      <c r="E39" s="7">
+        <f t="shared" si="0"/>
+        <v>15145</v>
+      </c>
+      <c r="F39" s="7">
+        <f t="shared" si="0"/>
+        <v>23864</v>
+      </c>
+      <c r="G39" s="7">
+        <f t="shared" si="0"/>
+        <v>39199</v>
+      </c>
+      <c r="H39" s="7">
+        <f t="shared" si="0"/>
+        <v>188845</v>
+      </c>
+      <c r="I39" s="7">
+        <f t="shared" si="0"/>
         <v>510064</v>
       </c>
-      <c r="K38" s="5" t="s">
+      <c r="K39" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L38" s="7">
-        <f t="shared" ref="L38:S38" si="4">MIN(B30, L30)</f>
+      <c r="L39" s="7">
+        <f t="shared" ref="L39:S39" si="4">MIN(B31, L31)</f>
         <v>4085</v>
       </c>
-      <c r="M38" s="7">
+      <c r="M39" s="7">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
-      <c r="N38" s="7">
+      <c r="N39" s="7">
         <f t="shared" si="4"/>
         <v>15657</v>
       </c>
-      <c r="O38" s="7">
+      <c r="O39" s="7">
         <f t="shared" si="4"/>
         <v>21730</v>
       </c>
-      <c r="P38" s="7">
+      <c r="P39" s="7">
         <f t="shared" si="4"/>
         <v>28454</v>
       </c>
-      <c r="Q38" s="7">
+      <c r="Q39" s="7">
         <f t="shared" si="4"/>
         <v>63292</v>
       </c>
-      <c r="R38" s="7">
+      <c r="R39" s="7">
         <f t="shared" si="4"/>
         <v>308037</v>
       </c>
-      <c r="S38" s="7">
+      <c r="S39" s="7">
         <f t="shared" si="4"/>
         <v>864129</v>
       </c>

</xml_diff>